<commit_message>
Remove unneeded parameters from driver
Begin work on Web Scraper
</commit_message>
<xml_diff>
--- a/InitalResults.xlsx
+++ b/InitalResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b75b1c6a55d49cb/College/JuniorYear/CS5140/Grade Data Mining Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\North\OneDrive\College\JuniorYear\CS5140\Grade Data Mining Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88F55C1E-5A13-444B-BE55-BDBCE20F0B6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{86C38A21-E582-4602-AFE5-88500E196588}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="26205" windowHeight="16260" activeTab="1" xr2:uid="{62ABDDFB-FB3E-4157-8F63-C5D156CD4AA8}"/>
+    <workbookView xWindow="4590" yWindow="4590" windowWidth="26205" windowHeight="16260" xr2:uid="{62ABDDFB-FB3E-4157-8F63-C5D156CD4AA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE41151D-FFC6-4B44-AA71-C58A2C9C4119}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,6 +1787,7 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1794,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56FB372-15BF-44C3-BF68-8C84E5F219EF}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>